<commit_message>
day 5 -all topics
</commit_message>
<xml_diff>
--- a/test_data/open_emr_data.xlsx
+++ b/test_data/open_emr_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji_Dinakaran\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\John Deere July 2023\RobotProject\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D4E1C68-F101-4F66-9715-A8D5B217D727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FDD3E8-BDC5-481E-A337-13456EBB669E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{8D4BF4D8-1241-49A8-8F9B-C9693C1579BC}"/>
+    <workbookView xWindow="2229" yWindow="2229" windowWidth="16457" windowHeight="9548" activeTab="1" xr2:uid="{8D4BF4D8-1241-49A8-8F9B-C9693C1579BC}"/>
   </bookViews>
   <sheets>
     <sheet name="VerifyValidLoginTemplate" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>${username}</t>
   </si>
@@ -62,6 +62,33 @@
   </si>
   <si>
     <t>receptionist</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>tag-id</t>
+  </si>
+  <si>
+    <t>tag-name</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>peter1</t>
+  </si>
+  <si>
+    <t>peter2</t>
   </si>
 </sst>
 </file>
@@ -415,7 +442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D23E0D5-4B5F-4831-95F8-B6CC49C21762}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -477,13 +504,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1217936E-CD5E-4F07-9D46-D92A7155ADBE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>